<commit_message>
activity sequence consistency: a tree structure would be appropriate
</commit_message>
<xml_diff>
--- a/template/activity_sequence.xlsx
+++ b/template/activity_sequence.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20373"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D3973B-12D9-4103-9131-5388E1DDC6B9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -67,7 +66,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -385,21 +384,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -410,7 +409,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -421,7 +420,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -432,7 +431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -443,7 +442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -454,7 +453,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -465,7 +464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -476,7 +475,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -487,7 +486,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -498,7 +497,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>

</xml_diff>